<commit_message>
Update DynaQ and NN
</commit_message>
<xml_diff>
--- a/results/all.xlsx
+++ b/results/all.xlsx
@@ -153,10 +153,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$101</c:f>
+              <c:f>Sheet1!$A$2:$A$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -300,285 +300,159 @@
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>47.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>48.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>49.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>52.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>53.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>54.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>55.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>56.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>57.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>58.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>59.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>60.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>61.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>62.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>63.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>65.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>66.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>67.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>68.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>69.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>70.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>71.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>72.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>73.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>74.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>75.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>76.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>77.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>78.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>79.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>80.0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>81.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>82.0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>83.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>84.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>85.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>86.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$101</c:f>
+              <c:f>Sheet1!$B$2:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0.22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.04</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0</c:v>
+                  <c:v>0.32</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.04</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="19">
+                  <c:v>0.14</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.14</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>0.0</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="29">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>0.02</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="33">
+                  <c:v>0.14</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.28</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.56</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>0.02</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.04</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.04</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="40">
                   <c:v>0.16</c:v>
                 </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>0.1</c:v>
                 </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.08</c:v>
-                </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.0</c:v>
+                  <c:v>0.46</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.04</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.0233333333333333</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -617,10 +491,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$101</c:f>
+              <c:f>Sheet1!$A$2:$A$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -764,133 +638,16 @@
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>47.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>48.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>49.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>52.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>53.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>54.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>55.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>56.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>57.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>58.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>59.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>60.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>61.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>62.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>63.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>65.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>66.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>67.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>68.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>69.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>70.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>71.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>72.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>73.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>74.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>75.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>76.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>77.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>78.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>79.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>80.0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>81.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>82.0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>83.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>84.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>85.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>86.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$101</c:f>
+              <c:f>Sheet1!$C$2:$C$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -1034,15 +791,6 @@
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>0.82</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.82</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.68</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.695</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1081,10 +829,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$101</c:f>
+              <c:f>Sheet1!$A$2:$A$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -1228,138 +976,21 @@
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>47.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>48.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>49.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>52.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>53.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>54.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>55.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>56.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>57.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>58.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>59.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>60.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>61.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>62.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>63.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>65.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>66.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>67.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>68.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>69.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>70.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>71.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>72.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>73.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>74.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>75.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>76.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>77.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>78.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>79.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>80.0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>81.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>82.0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>83.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>84.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>85.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>86.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$101</c:f>
+              <c:f>Sheet1!$D$2:$D$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
@@ -1368,145 +999,136 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.02</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.18</c:v>
+                  <c:v>0.76</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.02</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.2</c:v>
+                  <c:v>0.74</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.22</c:v>
+                  <c:v>0.58</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.1</c:v>
+                  <c:v>0.72</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.1</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.08</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.08</c:v>
+                  <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.08</c:v>
+                  <c:v>0.64</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.06</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.06</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.06</c:v>
+                  <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.26</c:v>
+                  <c:v>0.58</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.2</c:v>
+                  <c:v>0.72</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.18</c:v>
+                  <c:v>0.64</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.14</c:v>
+                  <c:v>0.64</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.28</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.12</c:v>
+                  <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.22</c:v>
+                  <c:v>0.76</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.28</c:v>
+                  <c:v>0.76</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.18</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.18</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.16</c:v>
+                  <c:v>0.72</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.2</c:v>
+                  <c:v>0.72</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.18</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.24</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.22</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.24</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.18</c:v>
+                  <c:v>0.76</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.26</c:v>
+                  <c:v>0.74</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.26</c:v>
+                  <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.0</c:v>
+                  <c:v>0.58</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.12</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.1</c:v>
+                  <c:v>0.72</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.08</c:v>
+                  <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.16</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.22</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.08</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.12</c:v>
+                  <c:v>0.72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1545,10 +1167,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$101</c:f>
+              <c:f>Sheet1!$A$2:$A$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -1692,133 +1314,160 @@
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>47.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>48.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>49.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>52.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>53.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>54.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>55.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>56.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>57.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>58.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>59.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>60.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>61.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>62.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>63.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>65.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>66.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>67.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>68.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>69.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>70.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>71.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>72.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>73.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>74.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>75.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>76.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>77.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>78.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>79.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>80.0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>81.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>82.0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>83.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>84.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>85.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>86.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$101</c:f>
+              <c:f>Sheet1!$E$2:$E$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+                <c:ptCount val="48"/>
+                <c:pt idx="0">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.28</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.28</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.28</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.42</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1832,11 +1481,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1653850784"/>
-        <c:axId val="1592025424"/>
+        <c:axId val="666567664"/>
+        <c:axId val="637422720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1653850784"/>
+        <c:axId val="666567664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50.0"/>
@@ -1949,12 +1598,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1592025424"/>
+        <c:crossAx val="637422720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1592025424"/>
+        <c:axId val="637422720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2067,7 +1716,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1653850784"/>
+        <c:crossAx val="666567664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3004,8 +2653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3032,7 +2681,7 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
@@ -3041,31 +2690,35 @@
       <c r="D2" s="1">
         <v>0</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2">
+        <v>0.36</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>A2+1</f>
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>0</v>
+      <c r="B3">
+        <v>0.1</v>
       </c>
       <c r="C3">
         <v>0.12</v>
       </c>
       <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1"/>
+        <v>0.08</v>
+      </c>
+      <c r="E3">
+        <v>0.38</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ref="A4:A67" si="0">A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="1">
-        <v>0</v>
+      <c r="B4">
+        <v>0.16</v>
       </c>
       <c r="C4">
         <v>0.26</v>
@@ -3073,15 +2726,17 @@
       <c r="D4" s="1">
         <v>0</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4">
+        <v>0.22</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B5" s="1">
-        <v>0</v>
+      <c r="B5">
+        <v>0.22</v>
       </c>
       <c r="C5">
         <v>0.7</v>
@@ -3089,31 +2744,35 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="1">
-        <v>0</v>
+      <c r="B6">
+        <v>0.04</v>
       </c>
       <c r="C6">
         <v>0.66</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>0.06</v>
+      </c>
+      <c r="E6">
+        <v>0.22</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B7" s="1">
-        <v>0.04</v>
+      <c r="B7">
+        <v>0.06</v>
       </c>
       <c r="C7">
         <v>0.56000000000000005</v>
@@ -3121,46 +2780,52 @@
       <c r="D7" s="1">
         <v>0</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="1">
-        <v>0</v>
+      <c r="B8">
+        <v>0.02</v>
       </c>
       <c r="C8">
         <v>0.5</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>0.16</v>
+      </c>
+      <c r="E8">
+        <v>0.26</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="1">
-        <v>0</v>
+      <c r="B9">
+        <v>0.32</v>
       </c>
       <c r="C9">
         <v>0.57999999999999996</v>
       </c>
       <c r="D9" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="E9" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0.26</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>0</v>
       </c>
       <c r="C10">
@@ -3169,663 +2834,747 @@
       <c r="D10" s="1">
         <v>0.02</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10">
+        <v>0.26</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="1">
-        <v>0.06</v>
+      <c r="B11">
+        <v>0.12</v>
       </c>
       <c r="C11">
         <v>0.84</v>
       </c>
       <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="E11">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" s="1">
-        <v>0.06</v>
+      <c r="B12">
+        <v>0.14000000000000001</v>
       </c>
       <c r="C12">
         <v>0.82</v>
       </c>
       <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="E12">
+        <v>0.36</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B13" s="1">
-        <v>0.04</v>
+      <c r="B13">
+        <v>0.2</v>
       </c>
       <c r="C13">
         <v>0.72</v>
       </c>
       <c r="D13" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="E13" s="1"/>
+        <v>0.68</v>
+      </c>
+      <c r="E13">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B14" s="1">
-        <v>0</v>
+      <c r="B14">
+        <v>0.14000000000000001</v>
       </c>
       <c r="C14">
         <v>0.7</v>
       </c>
       <c r="D14" s="1">
-        <v>0.18</v>
-      </c>
-      <c r="E14" s="1"/>
+        <v>0.76</v>
+      </c>
+      <c r="E14">
+        <v>0.26</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B15" s="1">
-        <v>0.02</v>
+      <c r="B15">
+        <v>0</v>
       </c>
       <c r="C15">
         <v>0.78</v>
       </c>
       <c r="D15" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="E15" s="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="E15">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B16" s="1">
-        <v>0</v>
+      <c r="B16">
+        <v>0.1</v>
       </c>
       <c r="C16">
         <v>0.7</v>
       </c>
       <c r="D16" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="E16" s="1"/>
+        <v>0.74</v>
+      </c>
+      <c r="E16">
+        <v>0.28000000000000003</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B17" s="1">
-        <v>0</v>
+      <c r="B17">
+        <v>0.32</v>
       </c>
       <c r="C17">
         <v>0.78</v>
       </c>
       <c r="D17" s="1">
-        <v>0.22</v>
-      </c>
-      <c r="E17" s="1"/>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E17">
+        <v>0.38</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B18" s="1">
-        <v>0</v>
+      <c r="B18">
+        <v>0.38</v>
       </c>
       <c r="C18">
         <v>0.8</v>
       </c>
       <c r="D18" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="E18" s="1"/>
+        <v>0.72</v>
+      </c>
+      <c r="E18">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B19" s="1">
-        <v>0</v>
+      <c r="B19">
+        <v>0.16</v>
       </c>
       <c r="C19">
         <v>0.7</v>
       </c>
       <c r="D19" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="E19" s="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="E19">
+        <v>0.38</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B20" s="1">
-        <v>0</v>
+      <c r="B20">
+        <v>0.06</v>
       </c>
       <c r="C20">
         <v>0.76</v>
       </c>
       <c r="D20" s="1">
-        <v>0.08</v>
-      </c>
-      <c r="E20" s="1"/>
+        <v>0.68</v>
+      </c>
+      <c r="E20">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B21" s="1">
-        <v>0</v>
+      <c r="B21">
+        <v>0.14000000000000001</v>
       </c>
       <c r="C21">
         <v>0.72</v>
       </c>
       <c r="D21" s="1">
-        <v>0.08</v>
-      </c>
-      <c r="E21" s="1"/>
+        <v>0.82</v>
+      </c>
+      <c r="E21">
+        <v>0.36</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B22" s="1">
-        <v>0</v>
+      <c r="B22">
+        <v>0.4</v>
       </c>
       <c r="C22">
         <v>0.74</v>
       </c>
       <c r="D22" s="1">
-        <v>0.08</v>
-      </c>
-      <c r="E22" s="1"/>
+        <v>0.64</v>
+      </c>
+      <c r="E22">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B23" s="1">
-        <v>0.02</v>
+      <c r="B23">
+        <v>0.14000000000000001</v>
       </c>
       <c r="C23">
         <v>0.68</v>
       </c>
       <c r="D23" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="E23" s="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="E23">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B24" s="1">
-        <v>0</v>
+      <c r="B24">
+        <v>0.08</v>
       </c>
       <c r="C24">
         <v>0.76</v>
       </c>
       <c r="D24" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="E24" s="1"/>
+        <v>0.68</v>
+      </c>
+      <c r="E24">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B25" s="1">
-        <v>0.02</v>
+      <c r="B25">
+        <v>0.08</v>
       </c>
       <c r="C25">
         <v>0.72</v>
       </c>
       <c r="D25" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="E25" s="1"/>
+        <v>0.66</v>
+      </c>
+      <c r="E25">
+        <v>0.22</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B26" s="1">
-        <v>0</v>
+      <c r="B26">
+        <v>0.26</v>
       </c>
       <c r="C26">
         <v>0.7</v>
       </c>
       <c r="D26" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="E26" s="1"/>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E26">
+        <v>0.36</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B27" s="1">
-        <v>0.02</v>
+      <c r="B27">
+        <v>0.2</v>
       </c>
       <c r="C27">
         <v>0.68</v>
       </c>
       <c r="D27" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="E27" s="1"/>
+        <v>0.72</v>
+      </c>
+      <c r="E27">
+        <v>0.36</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B28" s="1">
-        <v>0.06</v>
+      <c r="B28">
+        <v>0.36</v>
       </c>
       <c r="C28">
         <v>0.74</v>
       </c>
       <c r="D28" s="1">
-        <v>0.18</v>
-      </c>
-      <c r="E28" s="1"/>
+        <v>0.64</v>
+      </c>
+      <c r="E28">
+        <v>0.26</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B29" s="1">
-        <v>0.04</v>
+      <c r="B29">
+        <v>0.12</v>
       </c>
       <c r="C29">
         <v>0.78</v>
       </c>
       <c r="D29" s="1">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E29" s="1"/>
+        <v>0.64</v>
+      </c>
+      <c r="E29">
+        <v>0.46</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B30" s="1">
-        <v>0.04</v>
+      <c r="B30">
+        <v>0</v>
       </c>
       <c r="C30">
         <v>0.72</v>
       </c>
       <c r="D30" s="1">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="E30" s="1"/>
+        <v>0.68</v>
+      </c>
+      <c r="E30">
+        <v>0.26</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B31" s="1">
-        <v>0.02</v>
+      <c r="B31">
+        <v>0.2</v>
       </c>
       <c r="C31">
         <v>0.78</v>
       </c>
       <c r="D31" s="1">
-        <v>0.12</v>
-      </c>
-      <c r="E31" s="1"/>
+        <v>0.66</v>
+      </c>
+      <c r="E31">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B32" s="1">
-        <v>0</v>
+      <c r="B32">
+        <v>0.38</v>
       </c>
       <c r="C32">
         <v>0.68</v>
       </c>
       <c r="D32" s="1">
-        <v>0.22</v>
-      </c>
-      <c r="E32" s="1"/>
+        <v>0.76</v>
+      </c>
+      <c r="E32">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B33" s="1">
-        <v>0</v>
+      <c r="B33">
+        <v>0.2</v>
       </c>
       <c r="C33">
         <v>0.6</v>
       </c>
       <c r="D33" s="1">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="E33" s="1"/>
+        <v>0.76</v>
+      </c>
+      <c r="E33">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B34" s="1">
-        <v>0</v>
+      <c r="B34">
+        <v>0.02</v>
       </c>
       <c r="C34">
         <v>0.82</v>
       </c>
       <c r="D34" s="1">
-        <v>0.18</v>
-      </c>
-      <c r="E34" s="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="E34">
+        <v>0.46</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B35" s="1">
-        <v>0</v>
+      <c r="B35">
+        <v>0.14000000000000001</v>
       </c>
       <c r="C35">
         <v>0.74</v>
       </c>
       <c r="D35" s="1">
-        <v>0.18</v>
-      </c>
-      <c r="E35" s="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="E35">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B36" s="1">
-        <v>0</v>
+      <c r="B36">
+        <v>0.16</v>
       </c>
       <c r="C36">
         <v>0.74</v>
       </c>
       <c r="D36" s="1">
-        <v>0.16</v>
-      </c>
-      <c r="E36" s="1"/>
+        <v>0.72</v>
+      </c>
+      <c r="E36">
+        <v>0.26</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B37" s="1">
-        <v>0.02</v>
+      <c r="B37">
+        <v>0.18</v>
       </c>
       <c r="C37">
         <v>0.82</v>
       </c>
       <c r="D37" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="E37" s="1"/>
+        <v>0.72</v>
+      </c>
+      <c r="E37">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B38" s="1">
-        <v>0.16</v>
+      <c r="B38">
+        <v>0.28000000000000003</v>
       </c>
       <c r="C38">
         <v>0.72</v>
       </c>
       <c r="D38" s="1">
-        <v>0.18</v>
-      </c>
-      <c r="E38" s="1"/>
+        <v>0.54</v>
+      </c>
+      <c r="E38">
+        <v>0.34</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B39" s="1">
-        <v>0.02</v>
+      <c r="B39">
+        <v>0.22</v>
       </c>
       <c r="C39">
         <v>0.72</v>
       </c>
       <c r="D39" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="E39" s="1"/>
+        <v>0.68</v>
+      </c>
+      <c r="E39">
+        <v>0.38</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B40" s="1">
-        <v>0.06</v>
+      <c r="B40">
+        <v>0.56000000000000005</v>
       </c>
       <c r="C40">
         <v>0.72</v>
       </c>
       <c r="D40" s="1">
-        <v>0.22</v>
-      </c>
-      <c r="E40" s="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="E40">
+        <v>0.34</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B41" s="1">
-        <v>0</v>
+      <c r="B41">
+        <v>0.02</v>
       </c>
       <c r="C41">
         <v>0.8</v>
       </c>
       <c r="D41" s="1">
-        <v>0.24</v>
-      </c>
-      <c r="E41" s="1"/>
+        <v>0.78</v>
+      </c>
+      <c r="E41">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B42" s="1">
-        <v>0.1</v>
+      <c r="B42">
+        <v>0.16</v>
       </c>
       <c r="C42">
         <v>0.78</v>
       </c>
       <c r="D42" s="1">
-        <v>0.18</v>
-      </c>
-      <c r="E42" s="1"/>
+        <v>0.76</v>
+      </c>
+      <c r="E42">
+        <v>0.28000000000000003</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B43" s="1">
-        <v>0</v>
+      <c r="B43">
+        <v>0.42</v>
       </c>
       <c r="C43">
         <v>0.76</v>
       </c>
       <c r="D43" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="E43" s="1"/>
+        <v>0.74</v>
+      </c>
+      <c r="E43">
+        <v>0.22</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B44" s="1">
-        <v>0</v>
+      <c r="B44">
+        <v>0.8</v>
       </c>
       <c r="C44">
         <v>0.82</v>
       </c>
       <c r="D44" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="E44" s="1"/>
+        <v>0.66</v>
+      </c>
+      <c r="E44">
+        <v>0.46</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B45" s="1">
-        <v>0.2</v>
+      <c r="B45">
+        <v>0.12</v>
       </c>
       <c r="C45">
         <v>0.68</v>
       </c>
       <c r="D45" s="1">
-        <v>0</v>
-      </c>
-      <c r="E45" s="1"/>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E45">
+        <v>0.34</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B46" s="1">
-        <v>0</v>
+      <c r="B46">
+        <v>0.34</v>
       </c>
       <c r="C46">
         <v>0.78</v>
       </c>
       <c r="D46" s="1">
-        <v>0.12</v>
-      </c>
-      <c r="E46" s="1"/>
+        <v>0.68</v>
+      </c>
+      <c r="E46">
+        <v>0.28000000000000003</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B47" s="1">
-        <v>0.08</v>
+      <c r="B47">
+        <v>0.1</v>
       </c>
       <c r="C47">
         <v>0.72</v>
       </c>
       <c r="D47" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="E47" s="1"/>
+        <v>0.72</v>
+      </c>
+      <c r="E47">
+        <v>0.36</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="B48" s="1">
-        <v>0</v>
+      <c r="B48">
+        <v>0.46</v>
       </c>
       <c r="C48">
         <v>0.78</v>
       </c>
       <c r="D48" s="1">
-        <v>0.08</v>
-      </c>
-      <c r="E48" s="1"/>
+        <v>0.66</v>
+      </c>
+      <c r="E48">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="B49" s="1">
-        <v>0.04</v>
+      <c r="B49">
+        <v>0.12</v>
       </c>
       <c r="C49">
         <v>0.82</v>
       </c>
       <c r="D49" s="1">
-        <v>0.16</v>
-      </c>
-      <c r="E49" s="1"/>
+        <v>0.72</v>
+      </c>
+      <c r="E49">
+        <v>0.42</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B50" s="1">
-        <v>0</v>
+      <c r="B50">
+        <v>0.14000000000000001</v>
       </c>
       <c r="C50">
         <v>0.82</v>
       </c>
       <c r="D50" s="1">
-        <v>0.22</v>
-      </c>
-      <c r="E50" s="1"/>
+        <v>0.68</v>
+      </c>
+      <c r="E50">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="B51" s="1">
-        <v>0.06</v>
+      <c r="B51">
+        <v>0.44</v>
       </c>
       <c r="C51">
         <v>0.68</v>
       </c>
       <c r="D51" s="1">
-        <v>0.08</v>
-      </c>
-      <c r="E51" s="1"/>
+        <v>0.68</v>
+      </c>
+      <c r="E51">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
@@ -3834,7 +3583,7 @@
       </c>
       <c r="B52">
         <f t="shared" ref="B52:C52" si="1">AVERAGE(B2:B49)</f>
-        <v>2.3333333333333334E-2</v>
+        <v>0.19166666666666665</v>
       </c>
       <c r="C52">
         <f t="shared" si="1"/>

</xml_diff>